<commit_message>
handling files upload+ show admins lists + fixing admin bug
</commit_message>
<xml_diff>
--- a/public/uploads/medicines/approved_medicines.xlsx
+++ b/public/uploads/medicines/approved_medicines.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="34">
   <si>
     <t>ID</t>
   </si>
@@ -45,9 +45,6 @@
   </si>
   <si>
     <t>Tab</t>
-  </si>
-  <si>
-    <t>Bicalutamide</t>
   </si>
   <si>
     <t>Bleomycin</t>
@@ -372,7 +369,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -424,7 +421,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -629,7 +626,7 @@
   <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="67" workbookViewId="0">
-      <selection sqref="A1:L10"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -652,10 +649,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D1" s="13" t="s">
         <v>1</v>
@@ -664,25 +661,25 @@
         <v>2</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G1" s="13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H1" s="13" t="s">
         <v>3</v>
       </c>
       <c r="I1" s="13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J1" s="13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K1" s="14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L1" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="15" x14ac:dyDescent="0.25">
@@ -691,28 +688,28 @@
         <v>ActinVial500XXYY</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C2" s="8"/>
       <c r="D2" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E2" s="7">
         <v>500</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G2" s="7"/>
       <c r="H2" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J2" s="5"/>
       <c r="K2" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L2" s="11">
         <v>42688</v>
@@ -721,11 +718,9 @@
     <row r="3" spans="1:12" s="2" customFormat="1" ht="29.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="str">
         <f t="shared" ref="A3:A10" si="0">LEFT(B3,5)&amp;D3&amp;E3&amp;LEFT(H3,5)</f>
-        <v>AnastTab1Cipla</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>4</v>
-      </c>
+        <v>Tab1Cipla</v>
+      </c>
+      <c r="B3" s="12"/>
       <c r="C3" s="8"/>
       <c r="D3" s="4" t="s">
         <v>5</v>
@@ -734,18 +729,18 @@
         <v>1</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G3" s="7"/>
       <c r="H3" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J3" s="5"/>
       <c r="K3" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L3" s="11">
         <v>42688</v>
@@ -760,7 +755,7 @@
         <v>4</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>5</v>
@@ -769,18 +764,18 @@
         <v>1</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G4" s="7"/>
       <c r="H4" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="I4" s="5" t="s">
         <v>10</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>11</v>
       </c>
       <c r="J4" s="5"/>
       <c r="K4" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L4" s="11">
         <v>42688</v>
@@ -789,13 +784,13 @@
     <row r="5" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>AnastTab1Astra</v>
+        <v>AnastTab1</v>
       </c>
       <c r="B5" s="12" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>5</v>
@@ -804,18 +799,16 @@
         <v>1</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G5" s="7"/>
-      <c r="H5" s="8" t="s">
-        <v>10</v>
-      </c>
+      <c r="H5" s="8"/>
       <c r="I5" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J5" s="5"/>
       <c r="K5" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L5" s="11">
         <v>42688</v>
@@ -824,13 +817,11 @@
     <row r="6" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>AnastTab1Astra</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>4</v>
-      </c>
+        <v>Tab1Astra</v>
+      </c>
+      <c r="B6" s="12"/>
       <c r="C6" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>5</v>
@@ -839,18 +830,18 @@
         <v>1</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G6" s="7"/>
       <c r="H6" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J6" s="5"/>
       <c r="K6" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L6" s="11">
         <v>42688</v>
@@ -859,11 +850,9 @@
     <row r="7" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>BicalTab50AABB</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>6</v>
-      </c>
+        <v>Tab50</v>
+      </c>
+      <c r="B7" s="12"/>
       <c r="C7" s="8"/>
       <c r="D7" s="4" t="s">
         <v>5</v>
@@ -872,18 +861,16 @@
         <v>50</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G7" s="7"/>
-      <c r="H7" s="8" t="s">
-        <v>30</v>
-      </c>
+      <c r="H7" s="8"/>
       <c r="I7" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J7" s="5"/>
       <c r="K7" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L7" s="11">
         <v>42688</v>
@@ -895,28 +882,28 @@
         <v>BleomVial15AABB</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C8" s="8"/>
       <c r="D8" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E8" s="7">
         <v>15</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G8" s="7"/>
       <c r="H8" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J8" s="5"/>
       <c r="K8" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L8" s="11">
         <v>42688</v>
@@ -925,13 +912,11 @@
     <row r="9" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>CapecTab500Genen</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>8</v>
-      </c>
+        <v>Tab500</v>
+      </c>
+      <c r="B9" s="12"/>
       <c r="C9" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>5</v>
@@ -940,18 +925,16 @@
         <v>500</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G9" s="7"/>
-      <c r="H9" s="8" t="s">
-        <v>13</v>
-      </c>
+      <c r="H9" s="8"/>
       <c r="I9" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J9" s="5"/>
       <c r="K9" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L9" s="11">
         <v>42688</v>
@@ -963,10 +946,10 @@
         <v>CapecTab500Genen</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>5</v>
@@ -975,18 +958,18 @@
         <v>500</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G10" s="7"/>
       <c r="H10" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J10" s="5"/>
       <c r="K10" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L10" s="11">
         <v>42688</v>

</xml_diff>

<commit_message>
fixing medicines list issues
</commit_message>
<xml_diff>
--- a/public/uploads/medicines/approved_medicines.xlsx
+++ b/public/uploads/medicines/approved_medicines.xlsx
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9660"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9510"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="65">
   <si>
     <t>ID</t>
   </si>
@@ -77,6 +77,9 @@
     <t>COMMENTS</t>
   </si>
   <si>
+    <t>Bleomycin sulfate</t>
+  </si>
+  <si>
     <t>BLEO 15K</t>
   </si>
   <si>
@@ -98,6 +101,15 @@
     <t>https://www.ebs.tga.gov.au/servlet/xmlmillr6?dbid=ebs/PublicHTML/pdfStore.nsf&amp;docid=5C7F7743F1C4036BCA257F6B003CA203&amp;agid=(PrintDetailsPublic)&amp;actionid=1</t>
   </si>
   <si>
+    <t xml:space="preserve"> Blenoxane</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>Bristol Myers Squibb</t>
+  </si>
+  <si>
     <t>US FDA</t>
   </si>
   <si>
@@ -110,13 +122,103 @@
     <t>Discontiued</t>
   </si>
   <si>
-    <t>Kandom sulfate</t>
-  </si>
-  <si>
-    <t>mg</t>
-  </si>
-  <si>
-    <t>mf</t>
+    <t xml:space="preserve">Cipla Bleomycin </t>
+  </si>
+  <si>
+    <t>Cipla Australia Pty Ltd</t>
+  </si>
+  <si>
+    <t>30/30/2016</t>
+  </si>
+  <si>
+    <t>Fresenius kabi USA</t>
+  </si>
+  <si>
+    <t>28/01/2008</t>
+  </si>
+  <si>
+    <t>http://www.accessdata.fda.gov/scripts/cder/daf/index.cfm?event=overview.process&amp;ApplNo=065185</t>
+  </si>
+  <si>
+    <t>Hospira Bleomycin</t>
+  </si>
+  <si>
+    <t>Hospira Australia Pty Ltd</t>
+  </si>
+  <si>
+    <t>21/04/2005</t>
+  </si>
+  <si>
+    <t>https://www.ebs.tga.gov.au/servlet/xmlmillr6?dbid=ebs/PublicHTML/pdfStore.nsf&amp;docid=43D60045C53C5CE4CA2577DD00022002&amp;agid=(PrintDetailsPublic)&amp;actionid=1</t>
+  </si>
+  <si>
+    <t>Export only</t>
+  </si>
+  <si>
+    <t>10ml vial</t>
+  </si>
+  <si>
+    <t>10/03/2006</t>
+  </si>
+  <si>
+    <t>https://www.ebs.tga.gov.au/servlet/xmlmillr6?dbid=ebs/PublicHTML/pdfStore.nsf&amp;docid=5E46118FE9DF31BDCA2577DD00024310&amp;agid=(PrintDetailsPublic)&amp;actionid=1</t>
+  </si>
+  <si>
+    <t>DBL Bleomycin sulfate</t>
+  </si>
+  <si>
+    <t>12/01/2016</t>
+  </si>
+  <si>
+    <t>https://www.ebs.tga.gov.au/servlet/xmlmillr6?dbid=ebs/PublicHTML/pdfStore.nsf&amp;docid=2F6DC29BC6DF37AECA257F38003CA425&amp;agid=(PrintDetailsPublic)&amp;actionid=1</t>
+  </si>
+  <si>
+    <t>15/02/2006</t>
+  </si>
+  <si>
+    <t>https://www.ebs.tga.gov.au/servlet/xmlmillr6?dbid=ebs/PublicHTML/pdfStore.nsf&amp;docid=D87C9E57B9E7EA1BCA2577DD00024138&amp;agid=(PrintDetailsPublic)&amp;actionid=1</t>
+  </si>
+  <si>
+    <t>14/01/2008</t>
+  </si>
+  <si>
+    <t>https://www.ebs.tga.gov.au/servlet/xmlmillr6?dbid=ebs/PublicHTML/pdfStore.nsf&amp;docid=0976346121116FF4CA2577DD0002A25B&amp;agid=(PrintDetailsPublic)&amp;actionid=1</t>
+  </si>
+  <si>
+    <t>Bleo-Kyowa</t>
+  </si>
+  <si>
+    <t>5ml vial</t>
+  </si>
+  <si>
+    <t>Kyowa Kirin Ltd</t>
+  </si>
+  <si>
+    <t>UK</t>
+  </si>
+  <si>
+    <t>03/07/2006</t>
+  </si>
+  <si>
+    <t>http://www.medicines.org.uk/emc/search/?q=Bleomycin&amp;dt=2</t>
+  </si>
+  <si>
+    <t>Bleomycin</t>
+  </si>
+  <si>
+    <t>Pharmachemie BV</t>
+  </si>
+  <si>
+    <t>EMEA</t>
+  </si>
+  <si>
+    <t>12/03/2009</t>
+  </si>
+  <si>
+    <t>http://www.ema.europa.eu/ema/index.jsp?curl=pages/medicines/human/referrals/Bleomycin/human_referral_000010.jsp&amp;mid=WC0b01ac05805c516f</t>
+  </si>
+  <si>
+    <t>Discontinued in the US, in Europe discussion on cancer indication for drugs use</t>
   </si>
 </sst>
 </file>
@@ -126,10 +228,16 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -150,13 +258,37 @@
     </font>
     <font>
       <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -171,7 +303,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="-0.249977111117893"/>
+        <fgColor theme="8" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -185,33 +317,43 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="15" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 5" xfId="1"/>
   </cellStyles>
@@ -525,264 +667,805 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q5"/>
+  <dimension ref="A1:Q17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="M7" sqref="A1:Q17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="41.42578125" customWidth="1"/>
+    <col min="13" max="13" width="21" customWidth="1"/>
+    <col min="14" max="14" width="46.42578125" customWidth="1"/>
+    <col min="15" max="15" width="39.85546875" customWidth="1"/>
+    <col min="16" max="16" width="39" customWidth="1"/>
+    <col min="17" max="17" width="34.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="90" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="O1" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="P1" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="Q1" s="17" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="str">
-        <f t="shared" ref="A2:A5" si="0">LEFT(B2,5)&amp;D2&amp;E2&amp;LEFT(K2,5)</f>
-        <v>Kandovial15000Amnea</v>
-      </c>
-      <c r="B2" s="5" t="s">
+      <c r="A2" s="3" t="str">
+        <f t="shared" ref="A2:A11" si="0">LEFT(B2,5)&amp;D2&amp;E2&amp;LEFT(K2,5)</f>
+        <v>Bleomvial15000Amnea</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="5">
+        <v>15000</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4">
+        <v>1</v>
+      </c>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="O2" s="7">
+        <v>42768</v>
+      </c>
+      <c r="P2" s="7"/>
+      <c r="Q2" s="2"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>Bleomvial15000Amnea</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="5">
+        <v>15000</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4">
+        <v>10</v>
+      </c>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="N3" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="O3" s="7">
+        <v>42768</v>
+      </c>
+      <c r="P3" s="7"/>
+      <c r="Q3" s="2"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>Bleomvial15Brist</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="4">
+        <v>15</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="L4" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" s="7">
+      <c r="M4" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="N4" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="O4" s="7">
+        <v>42760</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q4" s="2"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>Bleomvial30Brist</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="4">
+        <v>30</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" s="2"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="L5" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="M5" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="N5" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="O5" s="7">
+        <v>42760</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q5" s="2"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>Bleomvial15000Cipla</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="5">
         <v>15000</v>
       </c>
-      <c r="F2" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="H2" s="6" t="s">
+      <c r="F6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4">
+        <v>1</v>
+      </c>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M6" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="N6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="O6" s="7">
+        <v>42768</v>
+      </c>
+      <c r="P6" s="7"/>
+      <c r="Q6" s="2"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>Bleomvial15000Cipla</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="5">
+        <v>15000</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4">
+        <v>10</v>
+      </c>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M7" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="N7" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="O7" s="7">
+        <v>42768</v>
+      </c>
+      <c r="P7" s="7"/>
+      <c r="Q7" s="2"/>
+    </row>
+    <row r="8" spans="1:17" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>Bleomvial15Frese</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="4">
+        <v>15</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L8" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="M8" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="N8" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="O8" s="7">
+        <v>42768</v>
+      </c>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
+    </row>
+    <row r="9" spans="1:17" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>Bleomvial30Frese</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="4">
         <v>30</v>
       </c>
-      <c r="I2" s="6">
+      <c r="F9" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L9" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="M9" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="N9" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="O9" s="7">
+        <v>42768</v>
+      </c>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>Bleomvial15Hospi</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="4">
+        <v>15</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4">
         <v>1</v>
       </c>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8" t="s">
+      <c r="J10" s="2"/>
+      <c r="K10" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M10" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="N10" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="O10" s="7">
+        <v>42760</v>
+      </c>
+      <c r="P10" s="11"/>
+      <c r="Q10" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>Bleomvial15Hospi</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="5">
+        <v>15</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G11" s="11"/>
+      <c r="H11" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="I11" s="4">
+        <v>1</v>
+      </c>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M11" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="N11" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="O11" s="7">
+        <v>42768</v>
+      </c>
+      <c r="P11" s="11"/>
+      <c r="Q11" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" ht="51.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="str">
+        <f>LEFT(B12,5)&amp;D6&amp;E6&amp;LEFT(K12,5)</f>
+        <v>Bleomvial15000Hospi</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" s="5">
+        <v>15000</v>
+      </c>
+      <c r="F12" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="L2" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="M2" s="9" t="s">
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4">
+        <v>10</v>
+      </c>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="L12" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="N2" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="O2" s="10">
+      <c r="M12" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="N12" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="O12" s="7">
         <v>42768</v>
       </c>
-      <c r="P2" s="10"/>
-      <c r="Q2" s="8"/>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>Kandovial15000Amnea</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" s="7">
+      <c r="P12" s="7"/>
+      <c r="Q12" s="2"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="str">
+        <f>LEFT(B13,5)&amp;D12&amp;E12&amp;LEFT(K13,5)</f>
+        <v>Bleomvial15000Hospi</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" s="5">
         <v>15000</v>
       </c>
-      <c r="F3" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="H3" s="6" t="s">
+      <c r="F13" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G13" s="11"/>
+      <c r="H13" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="I13" s="4">
+        <v>10</v>
+      </c>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M13" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="N13" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="O13" s="7">
+        <v>42768</v>
+      </c>
+      <c r="P13" s="11"/>
+      <c r="Q13" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="str">
+        <f>LEFT(B14,5)&amp;D13&amp;E13&amp;LEFT(K14,5)</f>
+        <v>Bleomvial15000Hospi</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" s="5">
+        <v>15000</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G14" s="11"/>
+      <c r="H14" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="I14" s="4">
+        <v>10</v>
+      </c>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M14" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="N14" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="O14" s="7">
+        <v>42768</v>
+      </c>
+      <c r="P14" s="11"/>
+      <c r="Q14" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="str">
+        <f t="shared" ref="A15:A17" si="1">LEFT(B15,5)&amp;D15&amp;E15&amp;LEFT(K15,5)</f>
+        <v>Bleomvial30Hospi</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E15" s="4">
         <v>30</v>
       </c>
-      <c r="I3" s="6">
+      <c r="F15" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4">
+        <v>1</v>
+      </c>
+      <c r="J15" s="12"/>
+      <c r="K15" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M15" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="N15" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="O15" s="7">
+        <v>42760</v>
+      </c>
+      <c r="P15" s="11"/>
+      <c r="Q15" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>Bleomvial15000Kyowa</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E16" s="5">
+        <v>15000</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G16" s="11"/>
+      <c r="H16" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="I16" s="4">
         <v>10</v>
       </c>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="L3" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="M3" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="N3" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="O3" s="10">
-        <v>42768</v>
-      </c>
-      <c r="P3" s="10"/>
-      <c r="Q3" s="8"/>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>Kandovial15000Amnea</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="7">
-        <v>15000</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="I4" s="6">
-        <v>90</v>
-      </c>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="L4" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="M4" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="N4" s="9" t="s">
+      <c r="J16" s="2"/>
+      <c r="K16" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="M16" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="N16" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="O16" s="7">
+        <v>42760</v>
+      </c>
+      <c r="P16" s="11"/>
+      <c r="Q16" s="2"/>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>Bleomvial15Pharm</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17" s="4">
+        <v>15</v>
+      </c>
+      <c r="F17" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="O4" s="10">
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="L17" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="M17" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="N17" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="O17" s="7">
         <v>42760</v>
       </c>
-      <c r="P4" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q4" s="8"/>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>Kandovial15000Amnea</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="7">
-        <v>15000</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="I5" s="6">
-        <v>78</v>
-      </c>
-      <c r="J5" s="8"/>
-      <c r="K5" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="L5" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="M5" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="N5" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="O5" s="10">
-        <v>42760</v>
-      </c>
-      <c r="P5" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q5" s="8"/>
+      <c r="P17" s="2"/>
+      <c r="Q17" s="2" t="s">
+        <v>64</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="N19" r:id="rId1" display="http://www.accessdata.fda.gov/scripts/cder/daf/index.cfm?event=overview.process&amp;ApplNo=064084"/>
+    <hyperlink ref="N9" r:id="rId2"/>
+    <hyperlink ref="N8" r:id="rId3"/>
+    <hyperlink ref="N16" r:id="rId4"/>
+    <hyperlink ref="N17" r:id="rId5"/>
+    <hyperlink ref="N15" r:id="rId6"/>
+    <hyperlink ref="N12" r:id="rId7"/>
+    <hyperlink ref="N10" r:id="rId8"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>